<commit_message>
Updated with results of multiprocessing
Updated the document, and the RS3 Archives.
</commit_message>
<xml_diff>
--- a/output/timeBuildBatch.xlsx
+++ b/output/timeBuildBatch.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>batchW1AC370-1</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t>total sec</t>
+  </si>
+  <si>
+    <t>total days</t>
+  </si>
+  <si>
+    <t>?? Dubious. Something's off</t>
   </si>
 </sst>
 </file>
@@ -1020,17 +1029,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D44F5F9-2B8D-4EA4-9247-F6F489A6D462}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1285,13 +1295,16 @@
         <f>SUM(F4:F12)</f>
         <v>6.4063074074074073</v>
       </c>
+      <c r="G14" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1304,46 +1317,46 @@
         <v>2.4129999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
       <c r="B18">
-        <f>MAX(timeBuildBatch!$H:$H)</f>
-        <v>37.564148466404106</v>
+        <f>MIN(timeBuildBatch!$H:$H)</f>
+        <v>0.41442188147534192</v>
       </c>
       <c r="C18">
         <f>MIN(timeBuildBatch!$G:$G)</f>
         <v>2.6621127879269259E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
       <c r="B19">
-        <f>MAX(timeBuildBatch!$H:$H)</f>
-        <v>37.564148466404106</v>
+        <f>AVERAGE(timeBuildBatch!$H:$H)</f>
+        <v>10.449699741657801</v>
       </c>
       <c r="C19">
         <f>AVERAGE(timeBuildBatch!$G:$G)</f>
         <v>0.39132160505339658</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
       <c r="B20">
-        <f>MAX(timeBuildBatch!$H:$H)</f>
-        <v>37.564148466404106</v>
+        <f>_xlfn.STDEV.P(timeBuildBatch!$H:$H)</f>
+        <v>9.6428014108932132</v>
       </c>
       <c r="C20">
         <f>_xlfn.STDEV.P(timeBuildBatch!$G:$G)</f>
         <v>0.67700182969832012</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1354,6 +1367,30 @@
       <c r="C21">
         <f>MEDIAN(timeBuildBatch!$G:$G)</f>
         <v>0.12350847457627119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <f>$C$14/B19</f>
+        <v>1308201.0333276105</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <f>B23/E23</f>
+        <v>15.141215663514011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>